<commit_message>
Added GPS time display
</commit_message>
<xml_diff>
--- a/Ford Cougar Cluster - LCD I2C decoding.xlsx
+++ b/Ford Cougar Cluster - LCD I2C decoding.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rse\source\repos\remiserriere\FordCougarEnhancedCluster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D514023C-2DBD-4D0B-9CE4-37928CE10F4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1E456E-DDDC-47AD-8700-4BBACD17D5F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82B46A02-7EB3-41E4-A60E-AC98783E40D9}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{82B46A02-7EB3-41E4-A60E-AC98783E40D9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Byte mapping" sheetId="1" r:id="rId1"/>
+    <sheet name="7-segment truth table" sheetId="2" r:id="rId2"/>
+    <sheet name="Digits 0-1-2-3 array builder" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$123</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Byte mapping'!$A$1:$L$123</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="57">
   <si>
     <t>d</t>
   </si>
@@ -158,11 +159,68 @@
   <si>
     <t>Not used</t>
   </si>
+  <si>
+    <t>Byte</t>
+  </si>
+  <si>
+    <t>uint64_t segmt a</t>
+  </si>
+  <si>
+    <t>uint64_t segmt b</t>
+  </si>
+  <si>
+    <t>uint64_t segmt c</t>
+  </si>
+  <si>
+    <t>uint64_t segmt d</t>
+  </si>
+  <si>
+    <t>uint64_t segmt e</t>
+  </si>
+  <si>
+    <t>uint64_t segmt f</t>
+  </si>
+  <si>
+    <t>uint64_t segmt g</t>
+  </si>
+  <si>
+    <t>uint64_t digit array</t>
+  </si>
+  <si>
+    <t>Digit 0</t>
+  </si>
+  <si>
+    <t>Digit 1</t>
+  </si>
+  <si>
+    <t>Digit 2</t>
+  </si>
+  <si>
+    <t>Digit 3</t>
+  </si>
+  <si>
+    <t>Time Sep</t>
+  </si>
+  <si>
+    <t>d0 string</t>
+  </si>
+  <si>
+    <t>d1 string</t>
+  </si>
+  <si>
+    <t>d2 string</t>
+  </si>
+  <si>
+    <t>d3 string</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="00"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -199,7 +257,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -233,11 +291,215 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -260,6 +522,66 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -281,16 +603,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>438972</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>38622</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>486597</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>19572</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -313,7 +635,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5676900" y="6200775"/>
+          <a:off x="5114925" y="10182225"/>
           <a:ext cx="5887272" cy="3743847"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -325,16 +647,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>400927</xdr:colOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>543802</xdr:colOff>
       <xdr:row>75</xdr:row>
-      <xdr:rowOff>105246</xdr:rowOff>
+      <xdr:rowOff>114771</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -357,7 +679,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10115550" y="10829925"/>
+          <a:off x="11477625" y="11029950"/>
           <a:ext cx="6287377" cy="3372321"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -689,8 +1011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01581DF9-FC2A-4B4C-BAC2-74C790D3C0E7}">
   <dimension ref="A1:L122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26:L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5031,19 +5353,15 @@
     <filterColumn colId="8" showButton="0"/>
   </autoFilter>
   <mergeCells count="32">
-    <mergeCell ref="C1:J1"/>
-    <mergeCell ref="A3:A10"/>
-    <mergeCell ref="A11:A18"/>
-    <mergeCell ref="A19:A26"/>
-    <mergeCell ref="A27:A34"/>
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="A35:A42"/>
-    <mergeCell ref="A43:A50"/>
-    <mergeCell ref="A51:A58"/>
-    <mergeCell ref="A59:A66"/>
-    <mergeCell ref="A115:A122"/>
-    <mergeCell ref="A75:A82"/>
+    <mergeCell ref="K118:L118"/>
+    <mergeCell ref="K122:L122"/>
+    <mergeCell ref="K95:L95"/>
+    <mergeCell ref="K97:L97"/>
+    <mergeCell ref="K99:L99"/>
+    <mergeCell ref="K100:L100"/>
+    <mergeCell ref="K101:L101"/>
+    <mergeCell ref="K103:L103"/>
+    <mergeCell ref="K104:L104"/>
     <mergeCell ref="K42:L42"/>
     <mergeCell ref="A83:A90"/>
     <mergeCell ref="A91:A98"/>
@@ -5054,15 +5372,19 @@
     <mergeCell ref="K110:L110"/>
     <mergeCell ref="K114:L114"/>
     <mergeCell ref="A67:A74"/>
-    <mergeCell ref="K118:L118"/>
-    <mergeCell ref="K122:L122"/>
-    <mergeCell ref="K95:L95"/>
-    <mergeCell ref="K97:L97"/>
-    <mergeCell ref="K99:L99"/>
-    <mergeCell ref="K100:L100"/>
-    <mergeCell ref="K101:L101"/>
-    <mergeCell ref="K103:L103"/>
-    <mergeCell ref="K104:L104"/>
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="A43:A50"/>
+    <mergeCell ref="A51:A58"/>
+    <mergeCell ref="A59:A66"/>
+    <mergeCell ref="A115:A122"/>
+    <mergeCell ref="A75:A82"/>
+    <mergeCell ref="C1:J1"/>
+    <mergeCell ref="A3:A10"/>
+    <mergeCell ref="A11:A18"/>
+    <mergeCell ref="A19:A26"/>
+    <mergeCell ref="A27:A34"/>
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="K26:L26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5763,4 +6085,1735 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8E7A3BC-C52C-410B-8D25-E64CE828C70A}">
+  <dimension ref="A1:BM12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AD28" sqref="AD28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="57" width="3" style="1" customWidth="1"/>
+    <col min="58" max="58" width="16.7109375" style="1" customWidth="1"/>
+    <col min="59" max="59" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="60" max="64" width="16.7109375" style="1" customWidth="1"/>
+    <col min="65" max="65" width="137.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="66" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="9">
+        <v>5</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="9">
+        <v>6</v>
+      </c>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="9">
+        <v>7</v>
+      </c>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="9">
+        <v>8</v>
+      </c>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="10"/>
+      <c r="AA1" s="10"/>
+      <c r="AB1" s="10"/>
+      <c r="AC1" s="11"/>
+      <c r="AD1" s="9">
+        <v>9</v>
+      </c>
+      <c r="AE1" s="10"/>
+      <c r="AF1" s="10"/>
+      <c r="AG1" s="10"/>
+      <c r="AH1" s="10"/>
+      <c r="AI1" s="10"/>
+      <c r="AJ1" s="11"/>
+      <c r="AK1" s="9">
+        <v>10</v>
+      </c>
+      <c r="AL1" s="10"/>
+      <c r="AM1" s="10"/>
+      <c r="AN1" s="10"/>
+      <c r="AO1" s="10"/>
+      <c r="AP1" s="10"/>
+      <c r="AQ1" s="11"/>
+      <c r="AR1" s="9">
+        <v>11</v>
+      </c>
+      <c r="AS1" s="10"/>
+      <c r="AT1" s="10"/>
+      <c r="AU1" s="10"/>
+      <c r="AV1" s="10"/>
+      <c r="AW1" s="10"/>
+      <c r="AX1" s="11"/>
+      <c r="AY1" s="9">
+        <v>13</v>
+      </c>
+      <c r="AZ1" s="10"/>
+      <c r="BA1" s="10"/>
+      <c r="BB1" s="10"/>
+      <c r="BC1" s="10"/>
+      <c r="BD1" s="10"/>
+      <c r="BE1" s="12"/>
+      <c r="BF1" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="BG1" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="BH1" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="BI1" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="BJ1" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="BK1" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="BL1" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="BM1" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q2" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="S2" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="U2" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="V2" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="W2" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="X2" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z2" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB2" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC2" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD2" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE2" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="AG2" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="AI2" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="AJ2" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK2" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="AL2" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM2" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="AN2" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO2" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="AP2" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="AQ2" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="AR2" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="AS2" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT2" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="AU2" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="AV2" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="AW2" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="AX2" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="AY2" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="AZ2" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="BA2" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="BB2" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="BC2" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="BD2" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="BE2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="BF2" s="17"/>
+      <c r="BG2" s="17"/>
+      <c r="BH2" s="17"/>
+      <c r="BI2" s="17"/>
+      <c r="BJ2" s="17"/>
+      <c r="BK2" s="17"/>
+      <c r="BL2" s="17"/>
+      <c r="BM2" s="17"/>
+    </row>
+    <row r="3" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="18"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="18">
+        <v>8</v>
+      </c>
+      <c r="Q3" s="19">
+        <v>4</v>
+      </c>
+      <c r="R3" s="19">
+        <v>2</v>
+      </c>
+      <c r="S3" s="19">
+        <v>1</v>
+      </c>
+      <c r="T3" s="19"/>
+      <c r="U3" s="19"/>
+      <c r="V3" s="20"/>
+      <c r="W3" s="18"/>
+      <c r="X3" s="19"/>
+      <c r="Y3" s="19"/>
+      <c r="Z3" s="19"/>
+      <c r="AA3" s="19">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="19">
+        <v>20</v>
+      </c>
+      <c r="AC3" s="20">
+        <v>10</v>
+      </c>
+      <c r="AD3" s="18"/>
+      <c r="AE3" s="19"/>
+      <c r="AF3" s="19"/>
+      <c r="AG3" s="19"/>
+      <c r="AH3" s="19"/>
+      <c r="AI3" s="19"/>
+      <c r="AJ3" s="20"/>
+      <c r="AK3" s="18"/>
+      <c r="AL3" s="19"/>
+      <c r="AM3" s="19"/>
+      <c r="AN3" s="19"/>
+      <c r="AO3" s="19"/>
+      <c r="AP3" s="19"/>
+      <c r="AQ3" s="20"/>
+      <c r="AR3" s="18"/>
+      <c r="AS3" s="19"/>
+      <c r="AT3" s="19"/>
+      <c r="AU3" s="19"/>
+      <c r="AV3" s="19"/>
+      <c r="AW3" s="19"/>
+      <c r="AX3" s="20"/>
+      <c r="AY3" s="18"/>
+      <c r="AZ3" s="19"/>
+      <c r="BA3" s="19"/>
+      <c r="BB3" s="19"/>
+      <c r="BC3" s="19"/>
+      <c r="BD3" s="19"/>
+      <c r="BE3" s="21"/>
+      <c r="BF3" s="22" t="str">
+        <f>B9&amp;I9&amp;P9&amp;W9&amp;AD9&amp;AK9&amp;AR9&amp;AY9</f>
+        <v>0000080000000000</v>
+      </c>
+      <c r="BG3" s="22" t="str">
+        <f t="shared" ref="BG3:BL3" si="0">C9&amp;J9&amp;Q9&amp;X9&amp;AE9&amp;AL9&amp;AS9&amp;AZ9</f>
+        <v>0000040000000000</v>
+      </c>
+      <c r="BH3" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>0000020000000000</v>
+      </c>
+      <c r="BI3" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>0000010000000000</v>
+      </c>
+      <c r="BJ3" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>0000000100000000</v>
+      </c>
+      <c r="BK3" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>0000002000000000</v>
+      </c>
+      <c r="BL3" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>0000001000000000</v>
+      </c>
+      <c r="BM3" s="22" t="str">
+        <f>"{0x"&amp;BF3&amp;", 0x"&amp;BG3&amp;", 0x"&amp;BH3&amp;", 0x"&amp;BI3&amp;", 0x"&amp;BJ3&amp;", 0x"&amp;BK3&amp;", 0x"&amp;BL3&amp;"}"</f>
+        <v>{0x0000080000000000, 0x0000040000000000, 0x0000020000000000, 0x0000010000000000, 0x0000000100000000, 0x0000002000000000, 0x0000001000000000}</v>
+      </c>
+    </row>
+    <row r="4" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="18"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="18">
+        <v>8</v>
+      </c>
+      <c r="J4" s="19">
+        <v>4</v>
+      </c>
+      <c r="K4" s="19">
+        <v>2</v>
+      </c>
+      <c r="L4" s="19">
+        <v>1</v>
+      </c>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="19"/>
+      <c r="T4" s="19"/>
+      <c r="U4" s="19">
+        <v>80</v>
+      </c>
+      <c r="V4" s="20">
+        <v>40</v>
+      </c>
+      <c r="W4" s="18"/>
+      <c r="X4" s="19"/>
+      <c r="Y4" s="19"/>
+      <c r="Z4" s="19"/>
+      <c r="AA4" s="19"/>
+      <c r="AB4" s="19"/>
+      <c r="AC4" s="20"/>
+      <c r="AD4" s="18"/>
+      <c r="AE4" s="19"/>
+      <c r="AF4" s="19"/>
+      <c r="AG4" s="19"/>
+      <c r="AH4" s="19">
+        <v>1</v>
+      </c>
+      <c r="AI4" s="19"/>
+      <c r="AJ4" s="20"/>
+      <c r="AK4" s="18"/>
+      <c r="AL4" s="19"/>
+      <c r="AM4" s="19"/>
+      <c r="AN4" s="19"/>
+      <c r="AO4" s="19"/>
+      <c r="AP4" s="19"/>
+      <c r="AQ4" s="20"/>
+      <c r="AR4" s="18"/>
+      <c r="AS4" s="19"/>
+      <c r="AT4" s="19"/>
+      <c r="AU4" s="19"/>
+      <c r="AV4" s="19"/>
+      <c r="AW4" s="19"/>
+      <c r="AX4" s="20"/>
+      <c r="AY4" s="18"/>
+      <c r="AZ4" s="19"/>
+      <c r="BA4" s="19"/>
+      <c r="BB4" s="19"/>
+      <c r="BC4" s="19"/>
+      <c r="BD4" s="19"/>
+      <c r="BE4" s="21"/>
+      <c r="BF4" s="22" t="str">
+        <f>B10&amp;I10&amp;P10&amp;W10&amp;AD10&amp;AK10&amp;AR10&amp;AY10</f>
+        <v>0008000000000000</v>
+      </c>
+      <c r="BG4" s="22" t="str">
+        <f>C10&amp;J10&amp;Q10&amp;X10&amp;AE10&amp;AL10&amp;AS10&amp;AZ10</f>
+        <v>0004000000000000</v>
+      </c>
+      <c r="BH4" s="22" t="str">
+        <f>D10&amp;K10&amp;R10&amp;Y10&amp;AF10&amp;AM10&amp;AT10&amp;BA10</f>
+        <v>0002000000000000</v>
+      </c>
+      <c r="BI4" s="22" t="str">
+        <f>E10&amp;L10&amp;S10&amp;Z10&amp;AG10&amp;AN10&amp;AU10&amp;BB10</f>
+        <v>0001000000000000</v>
+      </c>
+      <c r="BJ4" s="22" t="str">
+        <f>F10&amp;M10&amp;T10&amp;AA10&amp;AH10&amp;AO10&amp;AV10&amp;BC10</f>
+        <v>0000000001000000</v>
+      </c>
+      <c r="BK4" s="22" t="str">
+        <f>G10&amp;N10&amp;U10&amp;AB10&amp;AI10&amp;AP10&amp;AW10&amp;BD10</f>
+        <v>0000800000000000</v>
+      </c>
+      <c r="BL4" s="22" t="str">
+        <f>H10&amp;O10&amp;V10&amp;AC10&amp;AJ10&amp;AQ10&amp;AX10&amp;BE10</f>
+        <v>0000400000000000</v>
+      </c>
+      <c r="BM4" s="22" t="str">
+        <f>"{0x"&amp;BF4&amp;", 0x"&amp;BG4&amp;", 0x"&amp;BH4&amp;", 0x"&amp;BI4&amp;", 0x"&amp;BJ4&amp;", 0x"&amp;BK4&amp;", 0x"&amp;BL4&amp;"}"</f>
+        <v>{0x0008000000000000, 0x0004000000000000, 0x0002000000000000, 0x0001000000000000, 0x0000000001000000, 0x0000800000000000, 0x0000400000000000}</v>
+      </c>
+    </row>
+    <row r="5" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="18"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="18">
+        <v>80</v>
+      </c>
+      <c r="J5" s="19">
+        <v>40</v>
+      </c>
+      <c r="K5" s="19">
+        <v>20</v>
+      </c>
+      <c r="L5" s="19">
+        <v>10</v>
+      </c>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="19"/>
+      <c r="T5" s="19"/>
+      <c r="U5" s="19">
+        <v>20</v>
+      </c>
+      <c r="V5" s="20">
+        <v>10</v>
+      </c>
+      <c r="W5" s="18"/>
+      <c r="X5" s="19"/>
+      <c r="Y5" s="19"/>
+      <c r="Z5" s="19"/>
+      <c r="AA5" s="19"/>
+      <c r="AB5" s="19"/>
+      <c r="AC5" s="20"/>
+      <c r="AD5" s="18"/>
+      <c r="AE5" s="19"/>
+      <c r="AF5" s="19"/>
+      <c r="AG5" s="19"/>
+      <c r="AH5" s="19"/>
+      <c r="AI5" s="19"/>
+      <c r="AJ5" s="20"/>
+      <c r="AK5" s="18"/>
+      <c r="AL5" s="19"/>
+      <c r="AM5" s="19"/>
+      <c r="AN5" s="19"/>
+      <c r="AO5" s="19"/>
+      <c r="AP5" s="19"/>
+      <c r="AQ5" s="20"/>
+      <c r="AR5" s="18"/>
+      <c r="AS5" s="19"/>
+      <c r="AT5" s="19"/>
+      <c r="AU5" s="19"/>
+      <c r="AV5" s="19">
+        <v>1</v>
+      </c>
+      <c r="AW5" s="19"/>
+      <c r="AX5" s="20"/>
+      <c r="AY5" s="18"/>
+      <c r="AZ5" s="19"/>
+      <c r="BA5" s="19"/>
+      <c r="BB5" s="19"/>
+      <c r="BC5" s="19"/>
+      <c r="BD5" s="19"/>
+      <c r="BE5" s="21"/>
+      <c r="BF5" s="22" t="str">
+        <f>B11&amp;I11&amp;P11&amp;W11&amp;AD11&amp;AK11&amp;AR11&amp;AY11</f>
+        <v>0080000000000000</v>
+      </c>
+      <c r="BG5" s="22" t="str">
+        <f>C11&amp;J11&amp;Q11&amp;X11&amp;AE11&amp;AL11&amp;AS11&amp;AZ11</f>
+        <v>0040000000000000</v>
+      </c>
+      <c r="BH5" s="22" t="str">
+        <f>D11&amp;K11&amp;R11&amp;Y11&amp;AF11&amp;AM11&amp;AT11&amp;BA11</f>
+        <v>0020000000000000</v>
+      </c>
+      <c r="BI5" s="22" t="str">
+        <f>E11&amp;L11&amp;S11&amp;Z11&amp;AG11&amp;AN11&amp;AU11&amp;BB11</f>
+        <v>0010000000000000</v>
+      </c>
+      <c r="BJ5" s="22" t="str">
+        <f>F11&amp;M11&amp;T11&amp;AA11&amp;AH11&amp;AO11&amp;AV11&amp;BC11</f>
+        <v>0000000000000100</v>
+      </c>
+      <c r="BK5" s="22" t="str">
+        <f>G11&amp;N11&amp;U11&amp;AB11&amp;AI11&amp;AP11&amp;AW11&amp;BD11</f>
+        <v>0000200000000000</v>
+      </c>
+      <c r="BL5" s="22" t="str">
+        <f>H11&amp;O11&amp;V11&amp;AC11&amp;AJ11&amp;AQ11&amp;AX11&amp;BE11</f>
+        <v>0000100000000000</v>
+      </c>
+      <c r="BM5" s="22" t="str">
+        <f>"{0x"&amp;BF5&amp;", 0x"&amp;BG5&amp;", 0x"&amp;BH5&amp;", 0x"&amp;BI5&amp;", 0x"&amp;BJ5&amp;", 0x"&amp;BK5&amp;", 0x"&amp;BL5&amp;"}"</f>
+        <v>{0x0080000000000000, 0x0040000000000000, 0x0020000000000000, 0x0010000000000000, 0x0000000000000100, 0x0000200000000000, 0x0000100000000000}</v>
+      </c>
+    </row>
+    <row r="6" spans="1:65" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="23">
+        <v>8</v>
+      </c>
+      <c r="C6" s="24">
+        <v>4</v>
+      </c>
+      <c r="D6" s="24">
+        <v>2</v>
+      </c>
+      <c r="E6" s="24">
+        <v>1</v>
+      </c>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="24"/>
+      <c r="R6" s="24"/>
+      <c r="S6" s="24"/>
+      <c r="T6" s="24"/>
+      <c r="U6" s="24"/>
+      <c r="V6" s="25"/>
+      <c r="W6" s="23"/>
+      <c r="X6" s="24"/>
+      <c r="Y6" s="24"/>
+      <c r="Z6" s="24"/>
+      <c r="AA6" s="24"/>
+      <c r="AB6" s="24">
+        <v>80</v>
+      </c>
+      <c r="AC6" s="25">
+        <v>40</v>
+      </c>
+      <c r="AD6" s="23"/>
+      <c r="AE6" s="24"/>
+      <c r="AF6" s="24"/>
+      <c r="AG6" s="24"/>
+      <c r="AH6" s="24"/>
+      <c r="AI6" s="24"/>
+      <c r="AJ6" s="25"/>
+      <c r="AK6" s="23"/>
+      <c r="AL6" s="24"/>
+      <c r="AM6" s="24"/>
+      <c r="AN6" s="24"/>
+      <c r="AO6" s="24"/>
+      <c r="AP6" s="24"/>
+      <c r="AQ6" s="25"/>
+      <c r="AR6" s="23"/>
+      <c r="AS6" s="24"/>
+      <c r="AT6" s="24"/>
+      <c r="AU6" s="24"/>
+      <c r="AV6" s="24"/>
+      <c r="AW6" s="24"/>
+      <c r="AX6" s="25"/>
+      <c r="AY6" s="23"/>
+      <c r="AZ6" s="24"/>
+      <c r="BA6" s="24"/>
+      <c r="BB6" s="24"/>
+      <c r="BC6" s="24">
+        <v>1</v>
+      </c>
+      <c r="BD6" s="24"/>
+      <c r="BE6" s="26"/>
+      <c r="BF6" s="22" t="str">
+        <f>B12&amp;I12&amp;P12&amp;W12&amp;AD12&amp;AK12&amp;AR12&amp;AY12</f>
+        <v>0800000000000000</v>
+      </c>
+      <c r="BG6" s="22" t="str">
+        <f>C12&amp;J12&amp;Q12&amp;X12&amp;AE12&amp;AL12&amp;AS12&amp;AZ12</f>
+        <v>0400000000000000</v>
+      </c>
+      <c r="BH6" s="22" t="str">
+        <f>D12&amp;K12&amp;R12&amp;Y12&amp;AF12&amp;AM12&amp;AT12&amp;BA12</f>
+        <v>0200000000000000</v>
+      </c>
+      <c r="BI6" s="22" t="str">
+        <f>E12&amp;L12&amp;S12&amp;Z12&amp;AG12&amp;AN12&amp;AU12&amp;BB12</f>
+        <v>0100000000000000</v>
+      </c>
+      <c r="BJ6" s="22" t="str">
+        <f>F12&amp;M12&amp;T12&amp;AA12&amp;AH12&amp;AO12&amp;AV12&amp;BC12</f>
+        <v>0000000000000001</v>
+      </c>
+      <c r="BK6" s="22" t="str">
+        <f>G12&amp;N12&amp;U12&amp;AB12&amp;AI12&amp;AP12&amp;AW12&amp;BD12</f>
+        <v>0000008000000000</v>
+      </c>
+      <c r="BL6" s="22" t="str">
+        <f>H12&amp;O12&amp;V12&amp;AC12&amp;AJ12&amp;AQ12&amp;AX12&amp;BE12</f>
+        <v>0000004000000000</v>
+      </c>
+      <c r="BM6" s="22" t="str">
+        <f>"{0x"&amp;BF6&amp;", 0x"&amp;BG6&amp;", 0x"&amp;BH6&amp;", 0x"&amp;BI6&amp;", 0x"&amp;BJ6&amp;", 0x"&amp;BK6&amp;", 0x"&amp;BL6&amp;"}"</f>
+        <v>{0x0800000000000000, 0x0400000000000000, 0x0200000000000000, 0x0100000000000000, 0x0000000000000001, 0x0000008000000000, 0x0000004000000000}</v>
+      </c>
+    </row>
+    <row r="7" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="27"/>
+      <c r="O8" s="27"/>
+      <c r="P8" s="27"/>
+      <c r="Q8" s="27"/>
+      <c r="R8" s="27"/>
+      <c r="S8" s="27"/>
+      <c r="T8" s="27"/>
+      <c r="U8" s="27"/>
+      <c r="V8" s="27"/>
+      <c r="W8" s="27"/>
+      <c r="X8" s="27"/>
+      <c r="Y8" s="27"/>
+      <c r="Z8" s="27"/>
+      <c r="AA8" s="27"/>
+      <c r="AB8" s="27"/>
+      <c r="AC8" s="27"/>
+      <c r="AD8" s="27"/>
+      <c r="AE8" s="27"/>
+      <c r="AF8" s="27"/>
+      <c r="AG8" s="27"/>
+      <c r="AH8" s="27"/>
+      <c r="AI8" s="27"/>
+      <c r="AJ8" s="27"/>
+      <c r="AK8" s="27"/>
+      <c r="AL8" s="27"/>
+      <c r="AM8" s="27"/>
+      <c r="AN8" s="27"/>
+      <c r="AO8" s="27"/>
+      <c r="AP8" s="27"/>
+      <c r="AQ8" s="27"/>
+      <c r="AR8" s="27"/>
+      <c r="AS8" s="27"/>
+      <c r="AT8" s="27"/>
+      <c r="AU8" s="27"/>
+      <c r="AV8" s="27"/>
+      <c r="AW8" s="27"/>
+      <c r="AX8" s="27"/>
+      <c r="AY8" s="27"/>
+      <c r="AZ8" s="27"/>
+      <c r="BA8" s="27"/>
+      <c r="BB8" s="27"/>
+      <c r="BC8" s="27"/>
+      <c r="BD8" s="27"/>
+      <c r="BE8" s="27"/>
+    </row>
+    <row r="9" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="1" t="str">
+        <f>IF(B3&gt;0, TEXT(B3,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="C9" s="1" t="str">
+        <f t="shared" ref="C9:BE11" si="1">IF(C3&gt;0, TEXT(C3,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="D9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="E9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="F9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="G9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="H9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="I9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="J9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="K9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="L9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="M9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="N9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="O9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="P9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>08</v>
+      </c>
+      <c r="Q9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>04</v>
+      </c>
+      <c r="R9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>02</v>
+      </c>
+      <c r="S9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>01</v>
+      </c>
+      <c r="T9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="U9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="V9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="W9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="X9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="Y9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="Z9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="AA9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>01</v>
+      </c>
+      <c r="AB9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="AC9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="AD9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="AE9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="AF9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="AG9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="AH9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="AI9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="AJ9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="AK9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="AL9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="AM9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="AN9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="AO9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="AP9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="AQ9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="AR9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="AS9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="AT9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="AU9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="AV9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="AW9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="AX9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="AY9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="AZ9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="BA9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="BB9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="BC9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="BD9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="BE9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="10" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="1" t="str">
+        <f t="shared" ref="B10:BE11" si="2">IF(B4&gt;0, TEXT(B4,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="C10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="D10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="E10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="F10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="G10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="H10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="I10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>08</v>
+      </c>
+      <c r="J10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>04</v>
+      </c>
+      <c r="K10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>02</v>
+      </c>
+      <c r="L10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>01</v>
+      </c>
+      <c r="M10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="N10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="O10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="P10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="Q10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="R10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="S10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="T10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="U10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="V10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="W10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="X10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="Y10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="Z10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AA10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AB10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AC10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AD10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AE10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AF10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AG10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AH10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>01</v>
+      </c>
+      <c r="AI10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AJ10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AK10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="AL10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="AM10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="AN10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="AO10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="AP10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="AQ10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="AR10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AS10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AT10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AU10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AV10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AW10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AX10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AY10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AZ10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="BA10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="BB10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="BC10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="BD10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="BE10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="11" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="C11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="D11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="E11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="F11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="G11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="H11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="I11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="J11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="K11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="M11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="N11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="O11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="P11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="Q11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="R11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="S11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="T11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="U11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="V11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="W11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="X11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="Y11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="Z11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AA11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AB11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AC11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AD11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AE11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AF11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AG11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AH11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AI11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AJ11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AK11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="AL11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="AM11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="AN11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="AO11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="AP11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="AQ11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00</v>
+      </c>
+      <c r="AR11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AS11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AT11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AU11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AV11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>01</v>
+      </c>
+      <c r="AW11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AX11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AY11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="AZ11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="BA11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="BB11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="BC11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="BD11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+      <c r="BE11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="12" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="1" t="str">
+        <f>IF(B6&gt;0, TEXT(B6,"0#"), "00")</f>
+        <v>08</v>
+      </c>
+      <c r="C12" s="1" t="str">
+        <f>IF(C6&gt;0, TEXT(C6,"0#"), "00")</f>
+        <v>04</v>
+      </c>
+      <c r="D12" s="1" t="str">
+        <f>IF(D6&gt;0, TEXT(D6,"0#"), "00")</f>
+        <v>02</v>
+      </c>
+      <c r="E12" s="1" t="str">
+        <f>IF(E6&gt;0, TEXT(E6,"0#"), "00")</f>
+        <v>01</v>
+      </c>
+      <c r="F12" s="1" t="str">
+        <f>IF(F6&gt;0, TEXT(F6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="G12" s="1" t="str">
+        <f>IF(G6&gt;0, TEXT(G6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="H12" s="1" t="str">
+        <f>IF(H6&gt;0, TEXT(H6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="I12" s="1" t="str">
+        <f>IF(I6&gt;0, TEXT(I6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="J12" s="1" t="str">
+        <f>IF(J6&gt;0, TEXT(J6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="K12" s="1" t="str">
+        <f>IF(K6&gt;0, TEXT(K6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="L12" s="1" t="str">
+        <f>IF(L6&gt;0, TEXT(L6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="M12" s="1" t="str">
+        <f>IF(M6&gt;0, TEXT(M6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="N12" s="1" t="str">
+        <f>IF(N6&gt;0, TEXT(N6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="O12" s="1" t="str">
+        <f>IF(O6&gt;0, TEXT(O6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="P12" s="1" t="str">
+        <f>IF(P6&gt;0, TEXT(P6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="Q12" s="1" t="str">
+        <f>IF(Q6&gt;0, TEXT(Q6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="R12" s="1" t="str">
+        <f>IF(R6&gt;0, TEXT(R6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="S12" s="1" t="str">
+        <f>IF(S6&gt;0, TEXT(S6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="T12" s="1" t="str">
+        <f>IF(T6&gt;0, TEXT(T6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="U12" s="1" t="str">
+        <f>IF(U6&gt;0, TEXT(U6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="V12" s="1" t="str">
+        <f>IF(V6&gt;0, TEXT(V6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="W12" s="1" t="str">
+        <f>IF(W6&gt;0, TEXT(W6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="X12" s="1" t="str">
+        <f>IF(X6&gt;0, TEXT(X6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="Y12" s="1" t="str">
+        <f>IF(Y6&gt;0, TEXT(Y6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="Z12" s="1" t="str">
+        <f>IF(Z6&gt;0, TEXT(Z6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="AA12" s="1" t="str">
+        <f>IF(AA6&gt;0, TEXT(AA6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="AB12" s="1" t="str">
+        <f>IF(AB6&gt;0, TEXT(AB6,"0#"), "00")</f>
+        <v>80</v>
+      </c>
+      <c r="AC12" s="1" t="str">
+        <f>IF(AC6&gt;0, TEXT(AC6,"0#"), "00")</f>
+        <v>40</v>
+      </c>
+      <c r="AD12" s="1" t="str">
+        <f>IF(AD6&gt;0, TEXT(AD6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="AE12" s="1" t="str">
+        <f>IF(AE6&gt;0, TEXT(AE6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="AF12" s="1" t="str">
+        <f>IF(AF6&gt;0, TEXT(AF6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="AG12" s="1" t="str">
+        <f>IF(AG6&gt;0, TEXT(AG6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="AH12" s="1" t="str">
+        <f>IF(AH6&gt;0, TEXT(AH6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="AI12" s="1" t="str">
+        <f>IF(AI6&gt;0, TEXT(AI6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="AJ12" s="1" t="str">
+        <f>IF(AJ6&gt;0, TEXT(AJ6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="AK12" s="1" t="str">
+        <f>IF(AK6&gt;0, TEXT(AK6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="AL12" s="1" t="str">
+        <f>IF(AL6&gt;0, TEXT(AL6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="AM12" s="1" t="str">
+        <f>IF(AM6&gt;0, TEXT(AM6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="AN12" s="1" t="str">
+        <f>IF(AN6&gt;0, TEXT(AN6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="AO12" s="1" t="str">
+        <f>IF(AO6&gt;0, TEXT(AO6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="AP12" s="1" t="str">
+        <f>IF(AP6&gt;0, TEXT(AP6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="AQ12" s="1" t="str">
+        <f>IF(AQ6&gt;0, TEXT(AQ6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="AR12" s="1" t="str">
+        <f>IF(AR6&gt;0, TEXT(AR6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="AS12" s="1" t="str">
+        <f>IF(AS6&gt;0, TEXT(AS6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="AT12" s="1" t="str">
+        <f>IF(AT6&gt;0, TEXT(AT6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="AU12" s="1" t="str">
+        <f>IF(AU6&gt;0, TEXT(AU6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="AV12" s="1" t="str">
+        <f>IF(AV6&gt;0, TEXT(AV6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="AW12" s="1" t="str">
+        <f>IF(AW6&gt;0, TEXT(AW6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="AX12" s="1" t="str">
+        <f>IF(AX6&gt;0, TEXT(AX6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="AY12" s="1" t="str">
+        <f>IF(AY6&gt;0, TEXT(AY6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="AZ12" s="1" t="str">
+        <f>IF(AZ6&gt;0, TEXT(AZ6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="BA12" s="1" t="str">
+        <f>IF(BA6&gt;0, TEXT(BA6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="BB12" s="1" t="str">
+        <f>IF(BB6&gt;0, TEXT(BB6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="BC12" s="1" t="str">
+        <f>IF(BC6&gt;0, TEXT(BC6,"0#"), "00")</f>
+        <v>01</v>
+      </c>
+      <c r="BD12" s="1" t="str">
+        <f>IF(BD6&gt;0, TEXT(BD6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+      <c r="BE12" s="1" t="str">
+        <f>IF(BE6&gt;0, TEXT(BE6,"0#"), "00")</f>
+        <v>00</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="BJ1:BJ2"/>
+    <mergeCell ref="BK1:BK2"/>
+    <mergeCell ref="BL1:BL2"/>
+    <mergeCell ref="BM1:BM2"/>
+    <mergeCell ref="AR1:AX1"/>
+    <mergeCell ref="AY1:BE1"/>
+    <mergeCell ref="BF1:BF2"/>
+    <mergeCell ref="BG1:BG2"/>
+    <mergeCell ref="BH1:BH2"/>
+    <mergeCell ref="BI1:BI2"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="P1:V1"/>
+    <mergeCell ref="W1:AC1"/>
+    <mergeCell ref="AD1:AJ1"/>
+    <mergeCell ref="AK1:AQ1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>